<commit_message>
new set of results
</commit_message>
<xml_diff>
--- a/BMPs/summary_BMPs.xlsx
+++ b/BMPs/summary_BMPs.xlsx
@@ -497,16 +497,16 @@
         <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>2.128250210677612</v>
+        <v>2.622343602872005</v>
       </c>
       <c r="D2" t="n">
-        <v>2.086913019370249</v>
+        <v>2.152372601055987</v>
       </c>
       <c r="E2" t="n">
-        <v>1.725655264761822</v>
+        <v>1.792812421528958</v>
       </c>
       <c r="F2" t="n">
-        <v>1.401698057842716</v>
+        <v>1.369815210928913</v>
       </c>
     </row>
     <row r="3">
@@ -515,16 +515,16 @@
         <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>1.995107687833575</v>
+        <v>2.467743796815756</v>
       </c>
       <c r="D3" t="n">
-        <v>1.989606500868635</v>
+        <v>2.048974129801823</v>
       </c>
       <c r="E3" t="n">
-        <v>1.594836095759024</v>
+        <v>1.620336905513141</v>
       </c>
       <c r="F3" t="n">
-        <v>1.32703241487548</v>
+        <v>1.296394889716211</v>
       </c>
     </row>
     <row r="4">
@@ -533,16 +533,16 @@
         <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>1.887656807513339</v>
+        <v>2.320542303879344</v>
       </c>
       <c r="D4" t="n">
-        <v>1.92645141642838</v>
+        <v>1.95981595984354</v>
       </c>
       <c r="E4" t="n">
-        <v>1.454194627152703</v>
+        <v>1.42864171320842</v>
       </c>
       <c r="F4" t="n">
-        <v>1.289856862364087</v>
+        <v>1.258229492653228</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>1.796887086866436</v>
+        <v>2.230236732024127</v>
       </c>
       <c r="D5" t="n">
-        <v>1.859063975119397</v>
+        <v>1.871707064372008</v>
       </c>
       <c r="E5" t="n">
-        <v>1.330402803609853</v>
+        <v>1.303660677835469</v>
       </c>
       <c r="F5" t="n">
-        <v>1.256207838827099</v>
+        <v>1.212227701125545</v>
       </c>
     </row>
     <row r="6">
@@ -569,16 +569,16 @@
         <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>1.721375726137852</v>
+        <v>2.152898553230203</v>
       </c>
       <c r="D6" t="n">
-        <v>1.778567923675055</v>
+        <v>1.83018001984209</v>
       </c>
       <c r="E6" t="n">
-        <v>1.257505509752718</v>
+        <v>1.23237768401677</v>
       </c>
       <c r="F6" t="n">
-        <v>1.236813626332532</v>
+        <v>1.18414203421364</v>
       </c>
     </row>
     <row r="7">
@@ -587,16 +587,16 @@
         <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>1.691625595827066</v>
+        <v>2.112295704949706</v>
       </c>
       <c r="D7" t="n">
-        <v>1.73707055582982</v>
+        <v>1.777252250072877</v>
       </c>
       <c r="E7" t="n">
-        <v>1.237614390682806</v>
+        <v>1.211117753114425</v>
       </c>
       <c r="F7" t="n">
-        <v>1.232512697501235</v>
+        <v>1.176797248806555</v>
       </c>
     </row>
     <row r="8">
@@ -607,16 +607,16 @@
         <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>2.556049485397779</v>
+        <v>2.958156851108843</v>
       </c>
       <c r="D8" t="n">
-        <v>2.637322370919934</v>
+        <v>2.674168078258705</v>
       </c>
       <c r="E8" t="n">
-        <v>2.461011300555827</v>
+        <v>2.550467843302049</v>
       </c>
       <c r="F8" t="n">
-        <v>1.58663138815432</v>
+        <v>1.583334841892314</v>
       </c>
     </row>
     <row r="9">
@@ -625,16 +625,16 @@
         <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>2.344810441678146</v>
+        <v>2.752900061874218</v>
       </c>
       <c r="D9" t="n">
-        <v>2.487405758464518</v>
+        <v>2.583145584224332</v>
       </c>
       <c r="E9" t="n">
-        <v>2.213528365687691</v>
+        <v>2.273511081724153</v>
       </c>
       <c r="F9" t="n">
-        <v>1.515013711588414</v>
+        <v>1.493280646749689</v>
       </c>
     </row>
     <row r="10">
@@ -643,16 +643,16 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>2.202341682986782</v>
+        <v>2.582583693840313</v>
       </c>
       <c r="D10" t="n">
-        <v>2.393774343256014</v>
+        <v>2.475667281079886</v>
       </c>
       <c r="E10" t="n">
-        <v>2.071651206172283</v>
+        <v>2.100097495145042</v>
       </c>
       <c r="F10" t="n">
-        <v>1.457390227125151</v>
+        <v>1.427085768679523</v>
       </c>
     </row>
     <row r="11">
@@ -661,16 +661,16 @@
         <v>80</v>
       </c>
       <c r="C11" t="n">
-        <v>2.072322592532609</v>
+        <v>2.448407076303334</v>
       </c>
       <c r="D11" t="n">
-        <v>2.281485606700336</v>
+        <v>2.367729447486429</v>
       </c>
       <c r="E11" t="n">
-        <v>1.942093698646646</v>
+        <v>1.93213609938342</v>
       </c>
       <c r="F11" t="n">
-        <v>1.394879821076869</v>
+        <v>1.365686344900394</v>
       </c>
     </row>
     <row r="12">
@@ -679,16 +679,16 @@
         <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>1.981989809638347</v>
+        <v>2.372406859169245</v>
       </c>
       <c r="D12" t="n">
-        <v>2.177781811074698</v>
+        <v>2.309216619056827</v>
       </c>
       <c r="E12" t="n">
-        <v>1.862059804253548</v>
+        <v>1.811253008105346</v>
       </c>
       <c r="F12" t="n">
-        <v>1.370488147137758</v>
+        <v>1.354660165770392</v>
       </c>
     </row>
     <row r="13">
@@ -697,16 +697,16 @@
         <v>95</v>
       </c>
       <c r="C13" t="n">
-        <v>1.960545123465473</v>
+        <v>2.350073057069686</v>
       </c>
       <c r="D13" t="n">
-        <v>2.186167069461013</v>
+        <v>2.292150511552243</v>
       </c>
       <c r="E13" t="n">
-        <v>1.836603545636349</v>
+        <v>1.78281293013583</v>
       </c>
       <c r="F13" t="n">
-        <v>1.358837155795359</v>
+        <v>1.345185568082276</v>
       </c>
     </row>
     <row r="14">
@@ -717,16 +717,16 @@
         <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>3.626071174709379</v>
+        <v>4.186184925139913</v>
       </c>
       <c r="D14" t="n">
-        <v>3.654665919196305</v>
+        <v>3.705259749047888</v>
       </c>
       <c r="E14" t="n">
-        <v>3.877094481587054</v>
+        <v>3.997763106572068</v>
       </c>
       <c r="F14" t="n">
-        <v>2.024583758832521</v>
+        <v>7.516294411648735</v>
       </c>
     </row>
     <row r="15">
@@ -735,16 +735,16 @@
         <v>60</v>
       </c>
       <c r="C15" t="n">
-        <v>3.017787662175267</v>
+        <v>3.529960235733572</v>
       </c>
       <c r="D15" t="n">
-        <v>3.288948238514991</v>
+        <v>3.219004613924047</v>
       </c>
       <c r="E15" t="n">
-        <v>3.201376592234759</v>
+        <v>3.393555781299532</v>
       </c>
       <c r="F15" t="n">
-        <v>1.85781009874685</v>
+        <v>4.42378924772177</v>
       </c>
     </row>
     <row r="16">
@@ -753,16 +753,16 @@
         <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>2.646828088423014</v>
+        <v>3.047659905638771</v>
       </c>
       <c r="D16" t="n">
-        <v>2.974987475166435</v>
+        <v>3.022642601874604</v>
       </c>
       <c r="E16" t="n">
-        <v>2.910914259036906</v>
+        <v>2.860558958764877</v>
       </c>
       <c r="F16" t="n">
-        <v>1.710027344335425</v>
+        <v>4.818680357948059</v>
       </c>
     </row>
     <row r="17">
@@ -771,16 +771,16 @@
         <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>2.368963375809856</v>
+        <v>2.737747394635913</v>
       </c>
       <c r="D17" t="n">
-        <v>2.866211016409149</v>
+        <v>2.896606764649546</v>
       </c>
       <c r="E17" t="n">
-        <v>2.494671692856585</v>
+        <v>2.63564813082195</v>
       </c>
       <c r="F17" t="n">
-        <v>1.639941560695845</v>
+        <v>1.554774843480185</v>
       </c>
     </row>
     <row r="18">
@@ -789,16 +789,16 @@
         <v>90</v>
       </c>
       <c r="C18" t="n">
-        <v>2.192222180526486</v>
+        <v>2.604337145124109</v>
       </c>
       <c r="D18" t="n">
-        <v>2.832943125716342</v>
+        <v>2.841842788788624</v>
       </c>
       <c r="E18" t="n">
-        <v>2.403270203935166</v>
+        <v>2.508004185671087</v>
       </c>
       <c r="F18" t="n">
-        <v>1.607935060750413</v>
+        <v>5.621186927028381</v>
       </c>
     </row>
     <row r="19">
@@ -807,16 +807,16 @@
         <v>95</v>
       </c>
       <c r="C19" t="n">
-        <v>2.162310873767429</v>
+        <v>2.560096222394556</v>
       </c>
       <c r="D19" t="n">
-        <v>2.816724422958448</v>
+        <v>2.830459825793664</v>
       </c>
       <c r="E19" t="n">
-        <v>2.37525646028792</v>
+        <v>2.482622735449927</v>
       </c>
       <c r="F19" t="n">
-        <v>1.591685161910167</v>
+        <v>5.122441358375069</v>
       </c>
     </row>
   </sheetData>
@@ -883,16 +883,16 @@
         <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.9247585156949334</v>
+        <v>3.177543609231863</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.05833723007501225</v>
+        <v>-0.03978436966721279</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.188386729084457</v>
+        <v>-1.906796623613942</v>
       </c>
       <c r="F2" t="n">
-        <v>3.980535664791237</v>
+        <v>4.024350942332855</v>
       </c>
     </row>
     <row r="3">
@@ -901,16 +901,16 @@
         <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.232328874311179</v>
+        <v>2.969266681453517</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.2425975607994095</v>
+        <v>-0.2311813185200753</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.300835193678242</v>
+        <v>-2.204672901903208</v>
       </c>
       <c r="F3" t="n">
-        <v>3.963455687748642</v>
+        <v>3.898112040428388</v>
       </c>
     </row>
     <row r="4">
@@ -919,16 +919,16 @@
         <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.489368026605625</v>
+        <v>2.797527053072463</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4219204196155971</v>
+        <v>-0.3647913166204848</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.693327369938828</v>
+        <v>-2.465470268185995</v>
       </c>
       <c r="F4" t="n">
-        <v>3.952026826011608</v>
+        <v>3.847423945034185</v>
       </c>
     </row>
     <row r="5">
@@ -937,16 +937,16 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.66102391137705</v>
+        <v>2.669637651768938</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.5446952018282498</v>
+        <v>-0.5114753847105374</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.620922191418286</v>
+        <v>-2.634445552382329</v>
       </c>
       <c r="F5" t="n">
-        <v>3.880880531206778</v>
+        <v>3.790269888956434</v>
       </c>
     </row>
     <row r="6">
@@ -955,16 +955,16 @@
         <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.779913259825327</v>
+        <v>2.585888885530413</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.5835586839211715</v>
+        <v>-0.647116785714429</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.901817200628037</v>
+        <v>-2.751789613425808</v>
       </c>
       <c r="F6" t="n">
-        <v>3.839554957512372</v>
+        <v>3.784402992772982</v>
       </c>
     </row>
     <row r="7">
@@ -973,16 +973,16 @@
         <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.812683038495894</v>
+        <v>2.562268440366928</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.6455023440003598</v>
+        <v>-0.6694730001569413</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.929815880181872</v>
+        <v>-2.774240102855015</v>
       </c>
       <c r="F7" t="n">
-        <v>3.803913071444283</v>
+        <v>3.776778912376508</v>
       </c>
     </row>
     <row r="8">
@@ -993,16 +993,16 @@
         <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02701552577767018</v>
+        <v>3.576287246536824</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7444274685961068</v>
+        <v>0.7101759992094349</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2882677554363077</v>
+        <v>0.4955796383988253</v>
       </c>
       <c r="F8" t="n">
-        <v>4.699197867896714</v>
+        <v>4.56119207966749</v>
       </c>
     </row>
     <row r="9">
@@ -1011,16 +1011,16 @@
         <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.2046770237303293</v>
+        <v>3.365879330218584</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6206236364613635</v>
+        <v>0.5930360215155734</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2822166627695908</v>
+        <v>0.3411104034775309</v>
       </c>
       <c r="F9" t="n">
-        <v>4.657576181762174</v>
+        <v>4.443628372338141</v>
       </c>
     </row>
     <row r="10">
@@ -1029,16 +1029,16 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.3956986126311595</v>
+        <v>3.167043926109967</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5122198017623946</v>
+        <v>0.4626976785981737</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1291301290131357</v>
+        <v>0.2748553117789609</v>
       </c>
       <c r="F10" t="n">
-        <v>4.604658658536019</v>
+        <v>4.342497688574185</v>
       </c>
     </row>
     <row r="11">
@@ -1047,16 +1047,16 @@
         <v>80</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.5367673127563867</v>
+        <v>3.028202051342475</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5079411490026436</v>
+        <v>0.358776365922572</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01970969039633205</v>
+        <v>0.1225061720108877</v>
       </c>
       <c r="F11" t="n">
-        <v>4.585829619763748</v>
+        <v>4.252429318875691</v>
       </c>
     </row>
     <row r="12">
@@ -1065,16 +1065,16 @@
         <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.6377574683848887</v>
+        <v>2.951513286415557</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3793694343333723</v>
+        <v>0.2988633843486599</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.1669518423029156</v>
+        <v>0.05446543762244752</v>
       </c>
       <c r="F12" t="n">
-        <v>4.572140681916302</v>
+        <v>4.257505494064553</v>
       </c>
     </row>
     <row r="13">
@@ -1083,16 +1083,16 @@
         <v>95</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.6688130178389162</v>
+        <v>2.928314674622027</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3657608869776568</v>
+        <v>0.2874365223886469</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.07754923221361072</v>
+        <v>0.02043869269623629</v>
       </c>
       <c r="F13" t="n">
-        <v>4.536486670479349</v>
+        <v>4.247713267265833</v>
       </c>
     </row>
     <row r="14">
@@ -1103,16 +1103,16 @@
         <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8693626037354842</v>
+        <v>4.209049280856689</v>
       </c>
       <c r="D14" t="n">
-        <v>1.720538905642373</v>
+        <v>1.750553115997926</v>
       </c>
       <c r="E14" t="n">
-        <v>2.288603594426332</v>
+        <v>2.330955706507889</v>
       </c>
       <c r="F14" t="n">
-        <v>7.241458459147059</v>
+        <v>8.025967677761347</v>
       </c>
     </row>
     <row r="15">
@@ -1121,16 +1121,16 @@
         <v>60</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6172750589986176</v>
+        <v>3.953996322414121</v>
       </c>
       <c r="D15" t="n">
-        <v>1.671603355260392</v>
+        <v>1.761230797738574</v>
       </c>
       <c r="E15" t="n">
-        <v>2.18765360478696</v>
+        <v>2.237196927016431</v>
       </c>
       <c r="F15" t="n">
-        <v>7.156728964127302</v>
+        <v>7.540417283137299</v>
       </c>
     </row>
     <row r="16">
@@ -1139,16 +1139,16 @@
         <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4148906010702686</v>
+        <v>3.763337137567906</v>
       </c>
       <c r="D16" t="n">
-        <v>1.543311434173519</v>
+        <v>1.607766186132912</v>
       </c>
       <c r="E16" t="n">
-        <v>2.108743319084964</v>
+        <v>2.151255212171631</v>
       </c>
       <c r="F16" t="n">
-        <v>7.078588859622293</v>
+        <v>5.819938901545838</v>
       </c>
     </row>
     <row r="17">
@@ -1157,16 +1157,16 @@
         <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2792414331758642</v>
+        <v>3.618859103189898</v>
       </c>
       <c r="D17" t="n">
-        <v>1.544696135900817</v>
+        <v>1.560678251930118</v>
       </c>
       <c r="E17" t="n">
-        <v>2.051282067935396</v>
+        <v>2.142324663952231</v>
       </c>
       <c r="F17" t="n">
-        <v>7.091801476577789</v>
+        <v>4.867441673758091</v>
       </c>
     </row>
     <row r="18">
@@ -1175,16 +1175,16 @@
         <v>90</v>
       </c>
       <c r="C18" t="n">
-        <v>0.19074733131414</v>
+        <v>3.527151274981034</v>
       </c>
       <c r="D18" t="n">
-        <v>1.478120189674472</v>
+        <v>1.554208836938743</v>
       </c>
       <c r="E18" t="n">
-        <v>2.04731451033486</v>
+        <v>2.062012077394965</v>
       </c>
       <c r="F18" t="n">
-        <v>6.97916953785635</v>
+        <v>5.774437242774585</v>
       </c>
     </row>
     <row r="19">
@@ -1193,16 +1193,16 @@
         <v>95</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1655108010255418</v>
+        <v>3.501446753522099</v>
       </c>
       <c r="D19" t="n">
-        <v>1.484332543960984</v>
+        <v>1.538482330333837</v>
       </c>
       <c r="E19" t="n">
-        <v>2.004094138594419</v>
+        <v>2.049914574685602</v>
       </c>
       <c r="F19" t="n">
-        <v>7.008892553921756</v>
+        <v>5.738040569547072</v>
       </c>
     </row>
   </sheetData>
@@ -1269,16 +1269,16 @@
         <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>70.71184311025914</v>
+        <v>107.4296597082904</v>
       </c>
       <c r="D2" t="n">
-        <v>-161.6344694580706</v>
+        <v>-170.9490734061851</v>
       </c>
       <c r="E2" t="n">
-        <v>15.58565674517761</v>
+        <v>-46.16986736214476</v>
       </c>
       <c r="F2" t="n">
-        <v>34.48289404302395</v>
+        <v>29.61220544483864</v>
       </c>
     </row>
     <row r="3">
@@ -1287,16 +1287,16 @@
         <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>51.64695848558603</v>
+        <v>80.01418840355005</v>
       </c>
       <c r="D3" t="n">
-        <v>-164.8351004816257</v>
+        <v>-175.5594909888064</v>
       </c>
       <c r="E3" t="n">
-        <v>4.124671091143735</v>
+        <v>-38.23076950325969</v>
       </c>
       <c r="F3" t="n">
-        <v>1.000517992294195</v>
+        <v>-4.922154700028051</v>
       </c>
     </row>
     <row r="4">
@@ -1305,16 +1305,16 @@
         <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>35.5844190820013</v>
+        <v>57.62675698839772</v>
       </c>
       <c r="D4" t="n">
-        <v>-165.0081662974469</v>
+        <v>-176.6592724885395</v>
       </c>
       <c r="E4" t="n">
-        <v>5.491658640212472</v>
+        <v>-34.07260463176807</v>
       </c>
       <c r="F4" t="n">
-        <v>-24.64595347182345</v>
+        <v>-38.64690532393114</v>
       </c>
     </row>
     <row r="5">
@@ -1323,16 +1323,16 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>25.3286709062243</v>
+        <v>41.73340540086143</v>
       </c>
       <c r="D5" t="n">
-        <v>-161.8510648952189</v>
+        <v>-174.9432086932986</v>
       </c>
       <c r="E5" t="n">
-        <v>5.763472166283838</v>
+        <v>-38.63969579411587</v>
       </c>
       <c r="F5" t="n">
-        <v>-48.88696009273784</v>
+        <v>-48.89885406738815</v>
       </c>
     </row>
     <row r="6">
@@ -1341,16 +1341,16 @@
         <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>16.22549307324835</v>
+        <v>31.57732366730353</v>
       </c>
       <c r="D6" t="n">
-        <v>-164.260667096195</v>
+        <v>-173.1412857688555</v>
       </c>
       <c r="E6" t="n">
-        <v>6.037577705647596</v>
+        <v>-38.98735687509702</v>
       </c>
       <c r="F6" t="n">
-        <v>-65.39845732471579</v>
+        <v>-90.4157218435889</v>
       </c>
     </row>
     <row r="7">
@@ -1359,16 +1359,16 @@
         <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>13.01137243092424</v>
+        <v>28.15463027314234</v>
       </c>
       <c r="D7" t="n">
-        <v>-161.9400953451803</v>
+        <v>-174.9348211391927</v>
       </c>
       <c r="E7" t="n">
-        <v>6.036404563552524</v>
+        <v>-34.28704259331596</v>
       </c>
       <c r="F7" t="n">
-        <v>-69.49061133240215</v>
+        <v>-91.80752078820368</v>
       </c>
     </row>
     <row r="8">
@@ -1379,16 +1379,16 @@
         <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>120.7422418000725</v>
+        <v>156.4924928251481</v>
       </c>
       <c r="D8" t="n">
-        <v>109.2978652922738</v>
+        <v>64.19398041408618</v>
       </c>
       <c r="E8" t="n">
-        <v>231.7905218220137</v>
+        <v>225.0057266317329</v>
       </c>
       <c r="F8" t="n">
-        <v>88.06306299383024</v>
+        <v>84.50975636875324</v>
       </c>
     </row>
     <row r="9">
@@ -1397,16 +1397,16 @@
         <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>84.87136826918166</v>
+        <v>113.4578843523899</v>
       </c>
       <c r="D9" t="n">
-        <v>107.8890367632703</v>
+        <v>69.04200017046998</v>
       </c>
       <c r="E9" t="n">
-        <v>231.3632825382774</v>
+        <v>221.6319844641696</v>
       </c>
       <c r="F9" t="n">
-        <v>35.34061337801486</v>
+        <v>31.5568462593228</v>
       </c>
     </row>
     <row r="10">
@@ -1415,16 +1415,16 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>58.1342978640782</v>
+        <v>77.60461146999049</v>
       </c>
       <c r="D10" t="n">
-        <v>105.8835984362598</v>
+        <v>59.10119724568401</v>
       </c>
       <c r="E10" t="n">
-        <v>232.7715113981754</v>
+        <v>222.2795742563682</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.717458621428597</v>
+        <v>-2.177439049266614</v>
       </c>
     </row>
     <row r="11">
@@ -1433,16 +1433,16 @@
         <v>80</v>
       </c>
       <c r="C11" t="n">
-        <v>40.39432536968998</v>
+        <v>51.61839135927113</v>
       </c>
       <c r="D11" t="n">
-        <v>104.1754465680835</v>
+        <v>57.03780702584336</v>
       </c>
       <c r="E11" t="n">
-        <v>231.5082227618702</v>
+        <v>220.4671560861317</v>
       </c>
       <c r="F11" t="n">
-        <v>-28.14470964357532</v>
+        <v>-27.50425618612688</v>
       </c>
     </row>
     <row r="12">
@@ -1451,16 +1451,16 @@
         <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>27.6481705735581</v>
+        <v>37.10988979800545</v>
       </c>
       <c r="D12" t="n">
-        <v>107.5934387044587</v>
+        <v>58.62836346204453</v>
       </c>
       <c r="E12" t="n">
-        <v>225.3840571021746</v>
+        <v>219.112031937348</v>
       </c>
       <c r="F12" t="n">
-        <v>-44.92838459530953</v>
+        <v>-45.17961087476454</v>
       </c>
     </row>
     <row r="13">
@@ -1469,16 +1469,16 @@
         <v>95</v>
       </c>
       <c r="C13" t="n">
-        <v>23.3696001515067</v>
+        <v>32.36989815524446</v>
       </c>
       <c r="D13" t="n">
-        <v>107.5496783102915</v>
+        <v>56.80533239148262</v>
       </c>
       <c r="E13" t="n">
-        <v>229.0211226568645</v>
+        <v>220.1105575289303</v>
       </c>
       <c r="F13" t="n">
-        <v>-50.71274676941399</v>
+        <v>-51.40605853804824</v>
       </c>
     </row>
     <row r="14">
@@ -1489,16 +1489,16 @@
         <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>411.3070467954838</v>
+        <v>438.00642728003</v>
       </c>
       <c r="D14" t="n">
-        <v>566.0895739171643</v>
+        <v>509.6693379311161</v>
       </c>
       <c r="E14" t="n">
-        <v>626.3654658278791</v>
+        <v>525.8922274528072</v>
       </c>
       <c r="F14" t="n">
-        <v>363.18336187967</v>
+        <v>368.4414694810724</v>
       </c>
     </row>
     <row r="15">
@@ -1507,16 +1507,16 @@
         <v>60</v>
       </c>
       <c r="C15" t="n">
-        <v>265.5374814264113</v>
+        <v>286.6411065117536</v>
       </c>
       <c r="D15" t="n">
-        <v>567.6185811979818</v>
+        <v>501.5524677971714</v>
       </c>
       <c r="E15" t="n">
-        <v>566.1789840472832</v>
+        <v>512.7388996244135</v>
       </c>
       <c r="F15" t="n">
-        <v>210.8356607292894</v>
+        <v>213.9424078540109</v>
       </c>
     </row>
     <row r="16">
@@ -1525,16 +1525,16 @@
         <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>159.5579261643395</v>
+        <v>171.538325373381</v>
       </c>
       <c r="D16" t="n">
-        <v>600.1282634908285</v>
+        <v>511.5657045393625</v>
       </c>
       <c r="E16" t="n">
-        <v>619.4597752975451</v>
+        <v>520.774067300109</v>
       </c>
       <c r="F16" t="n">
-        <v>98.27724237239551</v>
+        <v>101.0910251704077</v>
       </c>
     </row>
     <row r="17">
@@ -1543,16 +1543,16 @@
         <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>84.49612345054784</v>
+        <v>93.29437651703002</v>
       </c>
       <c r="D17" t="n">
-        <v>599.1922720291655</v>
+        <v>511.8725731928532</v>
       </c>
       <c r="E17" t="n">
-        <v>615.638507187977</v>
+        <v>516.5485445287159</v>
       </c>
       <c r="F17" t="n">
-        <v>15.90390718938513</v>
+        <v>16.89823557386796</v>
       </c>
     </row>
     <row r="18">
@@ -1561,16 +1561,16 @@
         <v>90</v>
       </c>
       <c r="C18" t="n">
-        <v>40.24285740161969</v>
+        <v>46.55291311604739</v>
       </c>
       <c r="D18" t="n">
-        <v>602.4204197100242</v>
+        <v>510.0274130729304</v>
       </c>
       <c r="E18" t="n">
-        <v>558.1893522212285</v>
+        <v>506.7975653304317</v>
       </c>
       <c r="F18" t="n">
-        <v>-27.71897173100245</v>
+        <v>-26.76540981788858</v>
       </c>
     </row>
     <row r="19">
@@ -1579,16 +1579,16 @@
         <v>95</v>
       </c>
       <c r="C19" t="n">
-        <v>34.27629997813455</v>
+        <v>37.79185677047944</v>
       </c>
       <c r="D19" t="n">
-        <v>603.77304900845</v>
+        <v>511.1445933820991</v>
       </c>
       <c r="E19" t="n">
-        <v>612.1397049407593</v>
+        <v>518.2404452495438</v>
       </c>
       <c r="F19" t="n">
-        <v>-34.944101033237</v>
+        <v>-35.35592620018732</v>
       </c>
     </row>
   </sheetData>
@@ -1655,16 +1655,16 @@
         <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>-1178.800745216132</v>
+        <v>-80.93300756433213</v>
       </c>
       <c r="D2" t="n">
-        <v>-806.6970044694372</v>
+        <v>-757.1966177259908</v>
       </c>
       <c r="E2" t="n">
-        <v>-886.4394793326757</v>
+        <v>-791.8671208545053</v>
       </c>
       <c r="F2" t="n">
-        <v>-1484.436878802243</v>
+        <v>-1481.164561885753</v>
       </c>
     </row>
     <row r="3">
@@ -1673,16 +1673,16 @@
         <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>-1186.771534089187</v>
+        <v>-75.08284095990595</v>
       </c>
       <c r="D3" t="n">
-        <v>-906.5862544745519</v>
+        <v>-856.9401059815816</v>
       </c>
       <c r="E3" t="n">
-        <v>-971.3004309668515</v>
+        <v>-901.5787976304943</v>
       </c>
       <c r="F3" t="n">
-        <v>-1554.865992897519</v>
+        <v>-1548.126141576804</v>
       </c>
     </row>
     <row r="4">
@@ -1691,16 +1691,16 @@
         <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>-1192.289525237344</v>
+        <v>-70.81979555539878</v>
       </c>
       <c r="D4" t="n">
-        <v>-970.5859054895781</v>
+        <v>-930.2206057029123</v>
       </c>
       <c r="E4" t="n">
-        <v>-1035.471617339413</v>
+        <v>-977.0006499052721</v>
       </c>
       <c r="F4" t="n">
-        <v>-1605.987111346389</v>
+        <v>-1605.316076231936</v>
       </c>
     </row>
     <row r="5">
@@ -1709,16 +1709,16 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>-1188.91372085743</v>
+        <v>-66.61113142272887</v>
       </c>
       <c r="D5" t="n">
-        <v>-1012.60660198305</v>
+        <v>-982.8920636381758</v>
       </c>
       <c r="E5" t="n">
-        <v>-1088.00543396694</v>
+        <v>-1036.581254894904</v>
       </c>
       <c r="F5" t="n">
-        <v>-1644.620969254172</v>
+        <v>-1646.414680078871</v>
       </c>
     </row>
     <row r="6">
@@ -1727,16 +1727,16 @@
         <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>-1186.694285027966</v>
+        <v>-64.00145228219363</v>
       </c>
       <c r="D6" t="n">
-        <v>-1045.813220373054</v>
+        <v>-1030.894258805327</v>
       </c>
       <c r="E6" t="n">
-        <v>-1122.529826805241</v>
+        <v>-1074.999570201639</v>
       </c>
       <c r="F6" t="n">
-        <v>-1669.968329866965</v>
+        <v>-1673.399261691485</v>
       </c>
     </row>
     <row r="7">
@@ -1745,16 +1745,16 @@
         <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>-1185.837342430081</v>
+        <v>-62.97892799691954</v>
       </c>
       <c r="D7" t="n">
-        <v>-1060.649423541726</v>
+        <v>-1030.899433085953</v>
       </c>
       <c r="E7" t="n">
-        <v>-1131.983953587741</v>
+        <v>-1085.049471906633</v>
       </c>
       <c r="F7" t="n">
-        <v>-1678.539134665163</v>
+        <v>-1681.792750930526</v>
       </c>
     </row>
     <row r="8">
@@ -1765,16 +1765,16 @@
         <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>-997.7874745887541</v>
+        <v>-60.42308577715572</v>
       </c>
       <c r="D8" t="n">
-        <v>-644.8474274875023</v>
+        <v>-600.8513372340517</v>
       </c>
       <c r="E8" t="n">
-        <v>-641.034036095698</v>
+        <v>-584.4185733315876</v>
       </c>
       <c r="F8" t="n">
-        <v>-1249.350236745307</v>
+        <v>-1233.466485286343</v>
       </c>
     </row>
     <row r="9">
@@ -1783,16 +1783,16 @@
         <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>-992.7276294999183</v>
+        <v>-56.33059763461287</v>
       </c>
       <c r="D9" t="n">
-        <v>-722.4251182120345</v>
+        <v>-675.6420387036651</v>
       </c>
       <c r="E9" t="n">
-        <v>-706.9714204584012</v>
+        <v>-663.3919567223581</v>
       </c>
       <c r="F9" t="n">
-        <v>-1317.911914898072</v>
+        <v>-1301.148554351518</v>
       </c>
     </row>
     <row r="10">
@@ -1801,16 +1801,16 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>-993.6714600284561</v>
+        <v>-50.74692852206175</v>
       </c>
       <c r="D10" t="n">
-        <v>-787.8665540684917</v>
+        <v>-751.3006621524094</v>
       </c>
       <c r="E10" t="n">
-        <v>-762.3010838222057</v>
+        <v>-723.5853619289524</v>
       </c>
       <c r="F10" t="n">
-        <v>-1363.518649929636</v>
+        <v>-1350.13040345521</v>
       </c>
     </row>
     <row r="11">
@@ -1819,16 +1819,16 @@
         <v>80</v>
       </c>
       <c r="C11" t="n">
-        <v>-993.2189030194293</v>
+        <v>-47.456425395276</v>
       </c>
       <c r="D11" t="n">
-        <v>-822.6271236102438</v>
+        <v>-798.4006048734512</v>
       </c>
       <c r="E11" t="n">
-        <v>-811.2984199235495</v>
+        <v>-767.4070385893466</v>
       </c>
       <c r="F11" t="n">
-        <v>-1400.594062771264</v>
+        <v>-1385.402829390831</v>
       </c>
     </row>
     <row r="12">
@@ -1837,16 +1837,16 @@
         <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>-989.0636314291968</v>
+        <v>-45.15557654645145</v>
       </c>
       <c r="D12" t="n">
-        <v>-854.3917837786184</v>
+        <v>-828.5199526831867</v>
       </c>
       <c r="E12" t="n">
-        <v>-844.9287745192694</v>
+        <v>-804.7930228138418</v>
       </c>
       <c r="F12" t="n">
-        <v>-1422.221464030407</v>
+        <v>-1409.375447384455</v>
       </c>
     </row>
     <row r="13">
@@ -1855,16 +1855,16 @@
         <v>95</v>
       </c>
       <c r="C13" t="n">
-        <v>-987.8971650114096</v>
+        <v>-44.1311259397657</v>
       </c>
       <c r="D13" t="n">
-        <v>-864.8137738068423</v>
+        <v>-837.2314875851117</v>
       </c>
       <c r="E13" t="n">
-        <v>-845.9792051399677</v>
+        <v>-809.652993471131</v>
       </c>
       <c r="F13" t="n">
-        <v>-1429.294044914954</v>
+        <v>-1415.893854833625</v>
       </c>
     </row>
     <row r="14">
@@ -1875,16 +1875,16 @@
         <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>-835.2111568025846</v>
+        <v>-44.09613711799776</v>
       </c>
       <c r="D14" t="n">
-        <v>-502.3457865880794</v>
+        <v>-458.5911667135442</v>
       </c>
       <c r="E14" t="n">
-        <v>-495.0573786594626</v>
+        <v>-443.1269539172255</v>
       </c>
       <c r="F14" t="n">
-        <v>-1039.601867633009</v>
+        <v>-1038.219830213724</v>
       </c>
     </row>
     <row r="15">
@@ -1893,16 +1893,16 @@
         <v>60</v>
       </c>
       <c r="C15" t="n">
-        <v>-845.0288743864631</v>
+        <v>-39.56980893090507</v>
       </c>
       <c r="D15" t="n">
-        <v>-564.3237172270445</v>
+        <v>-531.0718350507482</v>
       </c>
       <c r="E15" t="n">
-        <v>-547.6000908771819</v>
+        <v>-488.4288937746577</v>
       </c>
       <c r="F15" t="n">
-        <v>-1083.243207625016</v>
+        <v>-1089.154267887503</v>
       </c>
     </row>
     <row r="16">
@@ -1911,16 +1911,16 @@
         <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>-845.7917101591075</v>
+        <v>-35.88459882019404</v>
       </c>
       <c r="D16" t="n">
-        <v>-613.2165355245442</v>
+        <v>-585.9988123076632</v>
       </c>
       <c r="E16" t="n">
-        <v>-600.1281404351834</v>
+        <v>-546.6070883231779</v>
       </c>
       <c r="F16" t="n">
-        <v>-1119.955356337274</v>
+        <v>-1129.359428272845</v>
       </c>
     </row>
     <row r="17">
@@ -1929,16 +1929,16 @@
         <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>-844.1549008782725</v>
+        <v>-33.25388379961492</v>
       </c>
       <c r="D17" t="n">
-        <v>-638.0606742346822</v>
+        <v>-633.83093193697</v>
       </c>
       <c r="E17" t="n">
-        <v>-637.7494999597986</v>
+        <v>-592.6663543202593</v>
       </c>
       <c r="F17" t="n">
-        <v>-1148.170522601763</v>
+        <v>-1158.925164780158</v>
       </c>
     </row>
     <row r="18">
@@ -1947,16 +1947,16 @@
         <v>90</v>
       </c>
       <c r="C18" t="n">
-        <v>-845.7224095044907</v>
+        <v>-31.35543874062113</v>
       </c>
       <c r="D18" t="n">
-        <v>-665.4157561736502</v>
+        <v>-645.5731067007855</v>
       </c>
       <c r="E18" t="n">
-        <v>-664.1924040101583</v>
+        <v>-615.3180842761971</v>
       </c>
       <c r="F18" t="n">
-        <v>-1167.055468322153</v>
+        <v>-1178.530209639965</v>
       </c>
     </row>
     <row r="19">
@@ -1965,16 +1965,16 @@
         <v>95</v>
       </c>
       <c r="C19" t="n">
-        <v>-846.2703441879165</v>
+        <v>-30.65932278024449</v>
       </c>
       <c r="D19" t="n">
-        <v>-673.9049732671065</v>
+        <v>-668.3325194137763</v>
       </c>
       <c r="E19" t="n">
-        <v>-670.9945765562913</v>
+        <v>-622.9578686840193</v>
       </c>
       <c r="F19" t="n">
-        <v>-1172.813525191859</v>
+        <v>-1184.543716965397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cornstover results after bug fix, exclude weird BMP results from lactic
</commit_message>
<xml_diff>
--- a/BMPs/summary_BMPs.xlsx
+++ b/BMPs/summary_BMPs.xlsx
@@ -497,7 +497,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>2.622343602872005</v>
+        <v>2.222894840016944</v>
       </c>
       <c r="D2" t="n">
         <v>2.152372601055987</v>
@@ -515,7 +515,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>2.467743796815756</v>
+        <v>2.081351166747502</v>
       </c>
       <c r="D3" t="n">
         <v>2.048974129801823</v>
@@ -533,7 +533,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>2.320542303879344</v>
+        <v>1.962467225995198</v>
       </c>
       <c r="D4" t="n">
         <v>1.95981595984354</v>
@@ -551,7 +551,7 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>2.230236732024127</v>
+        <v>1.844379580943132</v>
       </c>
       <c r="D5" t="n">
         <v>1.871707064372008</v>
@@ -569,7 +569,7 @@
         <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>2.152898553230203</v>
+        <v>1.763225476374728</v>
       </c>
       <c r="D6" t="n">
         <v>1.83018001984209</v>
@@ -578,7 +578,7 @@
         <v>1.23237768401677</v>
       </c>
       <c r="F6" t="n">
-        <v>1.18414203421364</v>
+        <v>1.183398211708029</v>
       </c>
     </row>
     <row r="7">
@@ -587,7 +587,7 @@
         <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>2.112295704949706</v>
+        <v>1.743076943634948</v>
       </c>
       <c r="D7" t="n">
         <v>1.777252250072877</v>
@@ -596,7 +596,7 @@
         <v>1.211117753114425</v>
       </c>
       <c r="F7" t="n">
-        <v>1.176797248806555</v>
+        <v>1.176159304169029</v>
       </c>
     </row>
     <row r="8">
@@ -607,7 +607,7 @@
         <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>2.958156851108843</v>
+        <v>2.573321818083491</v>
       </c>
       <c r="D8" t="n">
         <v>2.674168078258705</v>
@@ -625,7 +625,7 @@
         <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>2.752900061874218</v>
+        <v>2.360463260563568</v>
       </c>
       <c r="D9" t="n">
         <v>2.583145584224332</v>
@@ -643,7 +643,7 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>2.582583693840313</v>
+        <v>2.181077472300464</v>
       </c>
       <c r="D10" t="n">
         <v>2.475667281079886</v>
@@ -661,7 +661,7 @@
         <v>80</v>
       </c>
       <c r="C11" t="n">
-        <v>2.448407076303334</v>
+        <v>2.065482651075842</v>
       </c>
       <c r="D11" t="n">
         <v>2.367729447486429</v>
@@ -679,7 +679,7 @@
         <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>2.372406859169245</v>
+        <v>1.982096670058805</v>
       </c>
       <c r="D12" t="n">
         <v>2.309216619056827</v>
@@ -688,7 +688,7 @@
         <v>1.811253008105346</v>
       </c>
       <c r="F12" t="n">
-        <v>1.354660165770392</v>
+        <v>1.347707040680766</v>
       </c>
     </row>
     <row r="13">
@@ -697,7 +697,7 @@
         <v>95</v>
       </c>
       <c r="C13" t="n">
-        <v>2.350073057069686</v>
+        <v>1.965543273948365</v>
       </c>
       <c r="D13" t="n">
         <v>2.292150511552243</v>
@@ -706,7 +706,7 @@
         <v>1.78281293013583</v>
       </c>
       <c r="F13" t="n">
-        <v>1.345185568082276</v>
+        <v>1.340645131982352</v>
       </c>
     </row>
     <row r="14">
@@ -717,7 +717,7 @@
         <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>4.186184925139913</v>
+        <v>3.798504418416145</v>
       </c>
       <c r="D14" t="n">
         <v>3.705259749047888</v>
@@ -735,7 +735,7 @@
         <v>60</v>
       </c>
       <c r="C15" t="n">
-        <v>3.529960235733572</v>
+        <v>3.101354795070352</v>
       </c>
       <c r="D15" t="n">
         <v>3.219004613924047</v>
@@ -753,7 +753,7 @@
         <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>3.047659905638771</v>
+        <v>2.665321358710611</v>
       </c>
       <c r="D16" t="n">
         <v>3.022642601874604</v>
@@ -771,7 +771,7 @@
         <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>2.737747394635913</v>
+        <v>2.364075491314154</v>
       </c>
       <c r="D17" t="n">
         <v>2.896606764649546</v>
@@ -789,7 +789,7 @@
         <v>90</v>
       </c>
       <c r="C18" t="n">
-        <v>2.604337145124109</v>
+        <v>2.215306683784179</v>
       </c>
       <c r="D18" t="n">
         <v>2.841842788788624</v>
@@ -798,7 +798,7 @@
         <v>2.508004185671087</v>
       </c>
       <c r="F18" t="n">
-        <v>5.621186927028381</v>
+        <v>1.524438719629138</v>
       </c>
     </row>
     <row r="19">
@@ -807,7 +807,7 @@
         <v>95</v>
       </c>
       <c r="C19" t="n">
-        <v>2.560096222394556</v>
+        <v>2.181626032584568</v>
       </c>
       <c r="D19" t="n">
         <v>2.830459825793664</v>
@@ -816,7 +816,7 @@
         <v>2.482622735449927</v>
       </c>
       <c r="F19" t="n">
-        <v>5.122441358375069</v>
+        <v>1.512136622448377</v>
       </c>
     </row>
   </sheetData>
@@ -883,7 +883,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>3.177543609231863</v>
+        <v>-0.8633211588836323</v>
       </c>
       <c r="D2" t="n">
         <v>-0.03978436966721279</v>
@@ -901,7 +901,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>2.969266681453517</v>
+        <v>-1.17021592108262</v>
       </c>
       <c r="D3" t="n">
         <v>-0.2311813185200753</v>
@@ -919,7 +919,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>2.797527053072463</v>
+        <v>-1.425787129582262</v>
       </c>
       <c r="D4" t="n">
         <v>-0.3647913166204848</v>
@@ -937,7 +937,7 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>2.669637651768938</v>
+        <v>-1.600183394265429</v>
       </c>
       <c r="D5" t="n">
         <v>-0.5114753847105374</v>
@@ -955,7 +955,7 @@
         <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>2.585888885530413</v>
+        <v>-1.711878685561119</v>
       </c>
       <c r="D6" t="n">
         <v>-0.647116785714429</v>
@@ -964,7 +964,7 @@
         <v>-2.751789613425808</v>
       </c>
       <c r="F6" t="n">
-        <v>3.784402992772982</v>
+        <v>3.78092009393867</v>
       </c>
     </row>
     <row r="7">
@@ -973,7 +973,7 @@
         <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>2.562268440366928</v>
+        <v>-1.743504222895545</v>
       </c>
       <c r="D7" t="n">
         <v>-0.6694730001569413</v>
@@ -982,7 +982,7 @@
         <v>-2.774240102855015</v>
       </c>
       <c r="F7" t="n">
-        <v>3.776778912376508</v>
+        <v>3.773116407712585</v>
       </c>
     </row>
     <row r="8">
@@ -993,7 +993,7 @@
         <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>3.576287246536824</v>
+        <v>0.1341207350706173</v>
       </c>
       <c r="D8" t="n">
         <v>0.7101759992094349</v>
@@ -1011,7 +1011,7 @@
         <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>3.365879330218584</v>
+        <v>-0.1298203378663828</v>
       </c>
       <c r="D9" t="n">
         <v>0.5930360215155734</v>
@@ -1029,7 +1029,7 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>3.167043926109967</v>
+        <v>-0.3424236868735403</v>
       </c>
       <c r="D10" t="n">
         <v>0.4626976785981737</v>
@@ -1047,7 +1047,7 @@
         <v>80</v>
       </c>
       <c r="C11" t="n">
-        <v>3.028202051342475</v>
+        <v>-0.4929153403973364</v>
       </c>
       <c r="D11" t="n">
         <v>0.358776365922572</v>
@@ -1065,7 +1065,7 @@
         <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>2.951513286415557</v>
+        <v>-0.5985278638278291</v>
       </c>
       <c r="D12" t="n">
         <v>0.2988633843486599</v>
@@ -1074,7 +1074,7 @@
         <v>0.05446543762244752</v>
       </c>
       <c r="F12" t="n">
-        <v>4.257505494064553</v>
+        <v>4.214732559935982</v>
       </c>
     </row>
     <row r="13">
@@ -1083,7 +1083,7 @@
         <v>95</v>
       </c>
       <c r="C13" t="n">
-        <v>2.928314674622027</v>
+        <v>-0.6286930730025446</v>
       </c>
       <c r="D13" t="n">
         <v>0.2874365223886469</v>
@@ -1092,7 +1092,7 @@
         <v>0.02043869269623629</v>
       </c>
       <c r="F13" t="n">
-        <v>4.247713267265833</v>
+        <v>4.201840746793652</v>
       </c>
     </row>
     <row r="14">
@@ -1103,7 +1103,7 @@
         <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>4.209049280856689</v>
+        <v>0.8372937020526948</v>
       </c>
       <c r="D14" t="n">
         <v>1.750553115997926</v>
@@ -1121,7 +1121,7 @@
         <v>60</v>
       </c>
       <c r="C15" t="n">
-        <v>3.953996322414121</v>
+        <v>0.603239401840206</v>
       </c>
       <c r="D15" t="n">
         <v>1.761230797738574</v>
@@ -1139,7 +1139,7 @@
         <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>3.763337137567906</v>
+        <v>0.3943798609918671</v>
       </c>
       <c r="D16" t="n">
         <v>1.607766186132912</v>
@@ -1157,7 +1157,7 @@
         <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>3.618859103189898</v>
+        <v>0.2400555208856006</v>
       </c>
       <c r="D17" t="n">
         <v>1.560678251930118</v>
@@ -1175,7 +1175,7 @@
         <v>90</v>
       </c>
       <c r="C18" t="n">
-        <v>3.527151274981034</v>
+        <v>0.1517257797554393</v>
       </c>
       <c r="D18" t="n">
         <v>1.554208836938743</v>
@@ -1184,7 +1184,7 @@
         <v>2.062012077394965</v>
       </c>
       <c r="F18" t="n">
-        <v>5.774437242774585</v>
+        <v>4.844275418395246</v>
       </c>
     </row>
     <row r="19">
@@ -1193,7 +1193,7 @@
         <v>95</v>
       </c>
       <c r="C19" t="n">
-        <v>3.501446753522099</v>
+        <v>0.1266036772861589</v>
       </c>
       <c r="D19" t="n">
         <v>1.538482330333837</v>
@@ -1202,7 +1202,7 @@
         <v>2.049914574685602</v>
       </c>
       <c r="F19" t="n">
-        <v>5.738040569547072</v>
+        <v>4.832343476480743</v>
       </c>
     </row>
   </sheetData>
@@ -1269,7 +1269,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>107.4296597082904</v>
+        <v>73.48797373235243</v>
       </c>
       <c r="D2" t="n">
         <v>-170.9490734061851</v>
@@ -1287,7 +1287,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>80.01418840355005</v>
+        <v>51.30541777295414</v>
       </c>
       <c r="D3" t="n">
         <v>-175.5594909888064</v>
@@ -1305,7 +1305,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>57.62675698839772</v>
+        <v>35.51373386792045</v>
       </c>
       <c r="D4" t="n">
         <v>-176.6592724885395</v>
@@ -1323,7 +1323,7 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>41.73340540086143</v>
+        <v>25.3309272631408</v>
       </c>
       <c r="D5" t="n">
         <v>-174.9432086932986</v>
@@ -1341,7 +1341,7 @@
         <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>31.57732366730353</v>
+        <v>15.78157702493059</v>
       </c>
       <c r="D6" t="n">
         <v>-173.1412857688555</v>
@@ -1350,7 +1350,7 @@
         <v>-38.98735687509702</v>
       </c>
       <c r="F6" t="n">
-        <v>-90.4157218435889</v>
+        <v>-64.59234436812989</v>
       </c>
     </row>
     <row r="7">
@@ -1359,7 +1359,7 @@
         <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>28.15463027314234</v>
+        <v>12.8269031597602</v>
       </c>
       <c r="D7" t="n">
         <v>-174.9348211391927</v>
@@ -1368,7 +1368,7 @@
         <v>-34.28704259331596</v>
       </c>
       <c r="F7" t="n">
-        <v>-91.80752078820368</v>
+        <v>-69.08436617928808</v>
       </c>
     </row>
     <row r="8">
@@ -1379,7 +1379,7 @@
         <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>156.4924928251481</v>
+        <v>122.5309115816169</v>
       </c>
       <c r="D8" t="n">
         <v>64.19398041408618</v>
@@ -1397,7 +1397,7 @@
         <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>113.4578843523899</v>
+        <v>86.32869884435117</v>
       </c>
       <c r="D9" t="n">
         <v>69.04200017046998</v>
@@ -1415,7 +1415,7 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>77.60461146999049</v>
+        <v>58.48920111832051</v>
       </c>
       <c r="D10" t="n">
         <v>59.10119724568401</v>
@@ -1433,7 +1433,7 @@
         <v>80</v>
       </c>
       <c r="C11" t="n">
-        <v>51.61839135927113</v>
+        <v>40.70701943842687</v>
       </c>
       <c r="D11" t="n">
         <v>57.03780702584336</v>
@@ -1451,7 +1451,7 @@
         <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>37.10988979800545</v>
+        <v>27.44440028938203</v>
       </c>
       <c r="D12" t="n">
         <v>58.62836346204453</v>
@@ -1460,7 +1460,7 @@
         <v>219.112031937348</v>
       </c>
       <c r="F12" t="n">
-        <v>-45.17961087476454</v>
+        <v>-44.76062896011862</v>
       </c>
     </row>
     <row r="13">
@@ -1469,7 +1469,7 @@
         <v>95</v>
       </c>
       <c r="C13" t="n">
-        <v>32.36989815524446</v>
+        <v>23.48474074193043</v>
       </c>
       <c r="D13" t="n">
         <v>56.80533239148262</v>
@@ -1478,7 +1478,7 @@
         <v>220.1105575289303</v>
       </c>
       <c r="F13" t="n">
-        <v>-51.40605853804824</v>
+        <v>-50.41848222624078</v>
       </c>
     </row>
     <row r="14">
@@ -1489,7 +1489,7 @@
         <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>438.00642728003</v>
+        <v>405.9016141644476</v>
       </c>
       <c r="D14" t="n">
         <v>509.6693379311161</v>
@@ -1507,7 +1507,7 @@
         <v>60</v>
       </c>
       <c r="C15" t="n">
-        <v>286.6411065117536</v>
+        <v>264.3052443264097</v>
       </c>
       <c r="D15" t="n">
         <v>501.5524677971714</v>
@@ -1525,7 +1525,7 @@
         <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>171.538325373381</v>
+        <v>158.8977714287114</v>
       </c>
       <c r="D16" t="n">
         <v>511.5657045393625</v>
@@ -1543,7 +1543,7 @@
         <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>93.29437651703002</v>
+        <v>83.72441250124015</v>
       </c>
       <c r="D17" t="n">
         <v>511.8725731928532</v>
@@ -1561,7 +1561,7 @@
         <v>90</v>
       </c>
       <c r="C18" t="n">
-        <v>46.55291311604739</v>
+        <v>39.5382757341325</v>
       </c>
       <c r="D18" t="n">
         <v>510.0274130729304</v>
@@ -1570,7 +1570,7 @@
         <v>506.7975653304317</v>
       </c>
       <c r="F18" t="n">
-        <v>-26.76540981788858</v>
+        <v>-26.5366405259764</v>
       </c>
     </row>
     <row r="19">
@@ -1579,7 +1579,7 @@
         <v>95</v>
       </c>
       <c r="C19" t="n">
-        <v>37.79185677047944</v>
+        <v>34.35855151237573</v>
       </c>
       <c r="D19" t="n">
         <v>511.1445933820991</v>
@@ -1588,7 +1588,7 @@
         <v>518.2404452495438</v>
       </c>
       <c r="F19" t="n">
-        <v>-35.35592620018732</v>
+        <v>-35.10303027300269</v>
       </c>
     </row>
   </sheetData>
@@ -1655,7 +1655,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>-80.93300756433213</v>
+        <v>-1174.01788651092</v>
       </c>
       <c r="D2" t="n">
         <v>-757.1966177259908</v>
@@ -1673,7 +1673,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>-75.08284095990595</v>
+        <v>-1183.243328483077</v>
       </c>
       <c r="D3" t="n">
         <v>-856.9401059815816</v>
@@ -1691,7 +1691,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>-70.81979555539878</v>
+        <v>-1191.026939031916</v>
       </c>
       <c r="D4" t="n">
         <v>-930.2206057029123</v>
@@ -1709,7 +1709,7 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>-66.61113142272887</v>
+        <v>-1187.234103477948</v>
       </c>
       <c r="D5" t="n">
         <v>-982.8920636381758</v>
@@ -1727,7 +1727,7 @@
         <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>-64.00145228219363</v>
+        <v>-1184.77899704568</v>
       </c>
       <c r="D6" t="n">
         <v>-1030.894258805327</v>
@@ -1736,7 +1736,7 @@
         <v>-1074.999570201639</v>
       </c>
       <c r="F6" t="n">
-        <v>-1673.399261691485</v>
+        <v>-1678.572680181781</v>
       </c>
     </row>
     <row r="7">
@@ -1745,7 +1745,7 @@
         <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>-62.97892799691954</v>
+        <v>-1183.806756452163</v>
       </c>
       <c r="D7" t="n">
         <v>-1030.899433085953</v>
@@ -1754,7 +1754,7 @@
         <v>-1085.049471906633</v>
       </c>
       <c r="F7" t="n">
-        <v>-1681.792750930526</v>
+        <v>-1687.079993241087</v>
       </c>
     </row>
     <row r="8">
@@ -1765,7 +1765,7 @@
         <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>-60.42308577715572</v>
+        <v>-996.8199910720191</v>
       </c>
       <c r="D8" t="n">
         <v>-600.8513372340517</v>
@@ -1783,7 +1783,7 @@
         <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>-56.33059763461287</v>
+        <v>-993.1550244986875</v>
       </c>
       <c r="D9" t="n">
         <v>-675.6420387036651</v>
@@ -1801,7 +1801,7 @@
         <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>-50.74692852206175</v>
+        <v>-993.6949649005603</v>
       </c>
       <c r="D10" t="n">
         <v>-751.3006621524094</v>
@@ -1819,7 +1819,7 @@
         <v>80</v>
       </c>
       <c r="C11" t="n">
-        <v>-47.456425395276</v>
+        <v>-993.2773402229712</v>
       </c>
       <c r="D11" t="n">
         <v>-798.4006048734512</v>
@@ -1837,7 +1837,7 @@
         <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>-45.15557654645145</v>
+        <v>-990.1938840079094</v>
       </c>
       <c r="D12" t="n">
         <v>-828.5199526831867</v>
@@ -1846,7 +1846,7 @@
         <v>-804.7930228138418</v>
       </c>
       <c r="F12" t="n">
-        <v>-1409.375447384455</v>
+        <v>-1413.969643110279</v>
       </c>
     </row>
     <row r="13">
@@ -1855,7 +1855,7 @@
         <v>95</v>
       </c>
       <c r="C13" t="n">
-        <v>-44.1311259397657</v>
+        <v>-988.5667025547648</v>
       </c>
       <c r="D13" t="n">
         <v>-837.2314875851117</v>
@@ -1864,7 +1864,7 @@
         <v>-809.652993471131</v>
       </c>
       <c r="F13" t="n">
-        <v>-1415.893854833625</v>
+        <v>-1421.018183103475</v>
       </c>
     </row>
     <row r="14">
@@ -1875,7 +1875,7 @@
         <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>-44.09613711799776</v>
+        <v>-833.9761292759695</v>
       </c>
       <c r="D14" t="n">
         <v>-458.5911667135442</v>
@@ -1893,7 +1893,7 @@
         <v>60</v>
       </c>
       <c r="C15" t="n">
-        <v>-39.56980893090507</v>
+        <v>-845.3732885747194</v>
       </c>
       <c r="D15" t="n">
         <v>-531.0718350507482</v>
@@ -1911,7 +1911,7 @@
         <v>70</v>
       </c>
       <c r="C16" t="n">
-        <v>-35.88459882019404</v>
+        <v>-846.4284952975937</v>
       </c>
       <c r="D16" t="n">
         <v>-585.9988123076632</v>
@@ -1929,7 +1929,7 @@
         <v>80</v>
       </c>
       <c r="C17" t="n">
-        <v>-33.25388379961492</v>
+        <v>-844.819853559672</v>
       </c>
       <c r="D17" t="n">
         <v>-633.83093193697</v>
@@ -1947,7 +1947,7 @@
         <v>90</v>
       </c>
       <c r="C18" t="n">
-        <v>-31.35543874062113</v>
+        <v>-846.7576401731577</v>
       </c>
       <c r="D18" t="n">
         <v>-645.5731067007855</v>
@@ -1956,7 +1956,7 @@
         <v>-615.3180842761971</v>
       </c>
       <c r="F18" t="n">
-        <v>-1178.530209639965</v>
+        <v>-1179.894970869601</v>
       </c>
     </row>
     <row r="19">
@@ -1965,7 +1965,7 @@
         <v>95</v>
       </c>
       <c r="C19" t="n">
-        <v>-30.65932278024449</v>
+        <v>-846.5665255859478</v>
       </c>
       <c r="D19" t="n">
         <v>-668.3325194137763</v>
@@ -1974,7 +1974,7 @@
         <v>-622.9578686840193</v>
       </c>
       <c r="F19" t="n">
-        <v>-1184.543716965397</v>
+        <v>-1185.956082599678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>